<commit_message>
Feature create to search and filter summoners
Feature create to search and filter summoners by summonerName, summonerLevel, wins and losses
</commit_message>
<xml_diff>
--- a/res/uploads/Summoners.xlsx
+++ b/res/uploads/Summoners.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Id</t>
   </si>
@@ -89,6 +89,102 @@
   </si>
   <si>
     <t>cSZncIZPw32Fu4NV6R5i9PKbO-ri7BnmofL5EJVnjKplEAM</t>
+  </si>
+  <si>
+    <t>2bc01b6a-b331-4e8a-a094-7507ae7fa6bf</t>
+  </si>
+  <si>
+    <t>ThrekSor</t>
+  </si>
+  <si>
+    <t>uDfRght21EOdZ2s4EBmnszetb93pdaTxHDsZQ8n3QzLL2_M</t>
+  </si>
+  <si>
+    <t>x5s4POa3xnC9HoXrrz1vvCMjkUj9YBzftuEsrEtrZlnYDQ</t>
+  </si>
+  <si>
+    <t>a2e5ee7f-45a2-40e6-9740-4035167c0959</t>
+  </si>
+  <si>
+    <t>AndrewDiass</t>
+  </si>
+  <si>
+    <t>8f6gaNU2-GvZZt5JnO9RVtaIAIDLe6f1TVIPwDKpuY1Jl60</t>
+  </si>
+  <si>
+    <t>ZL-T-dfZdvqgwRyZBp6GzN_H3ZcKL6onpLdkjrRDgg-_w74</t>
+  </si>
+  <si>
+    <t>ba2c3634-2809-41b2-b2d0-639bd4c5c25a</t>
+  </si>
+  <si>
+    <t>BiliBoss</t>
+  </si>
+  <si>
+    <t>Ydvj2Yq0zsl85qcJ67dDL14XbXHh8uMn4KONjzLprKI</t>
+  </si>
+  <si>
+    <t>a_sIcNrytC9otnAGoXxT_WL9ZdL9n-UJYb4KHqX6cYph</t>
+  </si>
+  <si>
+    <t>a624d83a-4d81-4c59-8393-6729fd61dae2</t>
+  </si>
+  <si>
+    <t>DartSecond</t>
+  </si>
+  <si>
+    <t>8mFXXXaOuDsh632m5kBFjIN71mQo7sWHjS703w80Urbf0DM</t>
+  </si>
+  <si>
+    <t>-WMT4I99JbVdIC3ajBzfYN4C50hxTfR3f--qYJNmtVlMNQ</t>
+  </si>
+  <si>
+    <t>d087ee66-2163-4586-8a4c-e62fb63760bc</t>
+  </si>
+  <si>
+    <t>Devils Advocate</t>
+  </si>
+  <si>
+    <t>CAe5F92KMh3nBS-wEFZQuBkDPoDR6A9-H2O4UYyKhWM</t>
+  </si>
+  <si>
+    <t>yN8AgfGPRqBs7z-zwacwmF3W9nQ5IMZBacznV_T4nOVO</t>
+  </si>
+  <si>
+    <t>255128a2-2f0e-469b-987c-e68a52b57fd7</t>
+  </si>
+  <si>
+    <t>Gabrvxo</t>
+  </si>
+  <si>
+    <t>hICu0YjwVqqV-dj4elmavKbHFSBOjfRNMB36IfvjOFadO0scQWnsVDD5</t>
+  </si>
+  <si>
+    <t>j19n2pBr9HyUK3Bq46lBjeYlYIiKpzYv6g0IFH2WbKRFihE</t>
+  </si>
+  <si>
+    <t>80098f99-6e80-4f33-8c95-26c5889dc678</t>
+  </si>
+  <si>
+    <t>theKovac</t>
+  </si>
+  <si>
+    <t>HxFNVTVyNPuV7977R0ZLNTJRVVc2-C-nSmzbbonx4OeqVqI</t>
+  </si>
+  <si>
+    <t>kQOTOJNH3Izc_Jzzck4K5Bl4T5VbsMdPYCJoFrG16XNwaw</t>
+  </si>
+  <si>
+    <t>0b785189-776e-443c-bec9-8447f7150521</t>
+  </si>
+  <si>
+    <t>zRabelo</t>
+  </si>
+  <si>
+    <t>D4cBr1P8tvrUPxLC-XPQTgeFuxMiNW3_XB7IsY58GrbN5zw</t>
+  </si>
+  <si>
+    <t>Yljd_NnXEx6OgFmZwB6PQ8qYZrBUEaq14DfTCDeHM4sP2h0</t>
   </si>
 </sst>
 </file>
@@ -471,7 +567,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="35" customWidth="1"/>
@@ -625,6 +721,238 @@
         <v>32</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>331</v>
+      </c>
+      <c r="E6">
+        <v>777</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>327</v>
+      </c>
+      <c r="I6">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>262</v>
+      </c>
+      <c r="E7">
+        <v>4897</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>29</v>
+      </c>
+      <c r="I7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>42</v>
+      </c>
+      <c r="E8">
+        <v>1398</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>84</v>
+      </c>
+      <c r="E9">
+        <v>3836</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <v>373</v>
+      </c>
+      <c r="E10">
+        <v>4893</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10">
+        <v>184</v>
+      </c>
+      <c r="I10">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11">
+        <v>90</v>
+      </c>
+      <c r="E11">
+        <v>4397</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12">
+        <v>37</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13">
+        <v>133</v>
+      </c>
+      <c r="E13">
+        <v>4831</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13">
+        <v>63</v>
+      </c>
+      <c r="I13">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
instructions created for handling the API.
</commit_message>
<xml_diff>
--- a/res/uploads/Summoners.xlsx
+++ b/res/uploads/Summoners.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Id</t>
   </si>
@@ -40,58 +40,22 @@
     <t>Losses</t>
   </si>
   <si>
-    <t>238101e8-c19b-449c-8486-f6cc6ccfff00</t>
-  </si>
-  <si>
-    <t>THE WizzarD</t>
-  </si>
-  <si>
-    <t>JaB3SBtbohuD_j9AEoPTC2y3briWWJSplPOd_jh_ljCJAEM</t>
-  </si>
-  <si>
-    <t>NNx14OfVYeQ1jJZSMFszdtr132hlNjigFiigRBaQIcfv9Q</t>
+    <t>2cc9fd5b-a961-43b6-bf0b-9c68960ebbd9</t>
+  </si>
+  <si>
+    <t>Old Wolf King</t>
+  </si>
+  <si>
+    <t>O0Swjcn1aKrxrn0DlovVTNeu4bWiTvYXZeFRsgD_UGwVhNs</t>
+  </si>
+  <si>
+    <t>ArQcvoAbSEVftDHxS921HN2RMZFL7Sku9OATS98_4KA7GEA</t>
   </si>
   <si>
     <t>eff810ad-95b8-4a95-9475-d3c0da50bcce</t>
   </si>
   <si>
-    <t>805ad01e-1529-4f94-a4a9-9ed943ba3c75</t>
-  </si>
-  <si>
-    <t>Old Wolf King</t>
-  </si>
-  <si>
-    <t>O0Swjcn1aKrxrn0DlovVTNeu4bWiTvYXZeFRsgD_UGwVhNs</t>
-  </si>
-  <si>
-    <t>ArQcvoAbSEVftDHxS921HN2RMZFL7Sku9OATS98_4KA7GEA</t>
-  </si>
-  <si>
-    <t>088b94aa-2225-41fb-9197-9f6630c3422f</t>
-  </si>
-  <si>
-    <t>KnifeTheSkull</t>
-  </si>
-  <si>
-    <t>duryWWTOrWpp7wrWyiKPICFY59CvT1W5KfO329u3e6d6vQA</t>
-  </si>
-  <si>
-    <t>SjwN75jquERgi0ch1qfBF06Y-dVtHF5HerErgWj6_2LVbw</t>
-  </si>
-  <si>
-    <t>709c99fb-8f9f-4d42-ae5e-003c2c0f1a1e</t>
-  </si>
-  <si>
-    <t>Risos12</t>
-  </si>
-  <si>
-    <t>Rc-E8fiKtvu5kTiryraaEh2IGOAAS9r8uIzboKBSnWQDQELrmOqTkqNp</t>
-  </si>
-  <si>
-    <t>cSZncIZPw32Fu4NV6R5i9PKbO-ri7BnmofL5EJVnjKplEAM</t>
-  </si>
-  <si>
-    <t>2bc01b6a-b331-4e8a-a094-7507ae7fa6bf</t>
+    <t>888d495a-d2c5-48e3-b19b-7b8979baa2ad</t>
   </si>
   <si>
     <t>ThrekSor</t>
@@ -103,7 +67,7 @@
     <t>x5s4POa3xnC9HoXrrz1vvCMjkUj9YBzftuEsrEtrZlnYDQ</t>
   </si>
   <si>
-    <t>a2e5ee7f-45a2-40e6-9740-4035167c0959</t>
+    <t>5117f20c-14ab-4f55-848f-0720d18aec54</t>
   </si>
   <si>
     <t>AndrewDiass</t>
@@ -115,7 +79,7 @@
     <t>ZL-T-dfZdvqgwRyZBp6GzN_H3ZcKL6onpLdkjrRDgg-_w74</t>
   </si>
   <si>
-    <t>ba2c3634-2809-41b2-b2d0-639bd4c5c25a</t>
+    <t>3e3e8aba-5d42-4cbc-8b9e-206ead6ab293</t>
   </si>
   <si>
     <t>BiliBoss</t>
@@ -127,7 +91,7 @@
     <t>a_sIcNrytC9otnAGoXxT_WL9ZdL9n-UJYb4KHqX6cYph</t>
   </si>
   <si>
-    <t>a624d83a-4d81-4c59-8393-6729fd61dae2</t>
+    <t>3f69ac42-6d11-4597-9215-b14981a84b0e</t>
   </si>
   <si>
     <t>DartSecond</t>
@@ -139,7 +103,7 @@
     <t>-WMT4I99JbVdIC3ajBzfYN4C50hxTfR3f--qYJNmtVlMNQ</t>
   </si>
   <si>
-    <t>d087ee66-2163-4586-8a4c-e62fb63760bc</t>
+    <t>c566a10b-3992-425c-95a4-df010f1ea34c</t>
   </si>
   <si>
     <t>Devils Advocate</t>
@@ -151,7 +115,7 @@
     <t>yN8AgfGPRqBs7z-zwacwmF3W9nQ5IMZBacznV_T4nOVO</t>
   </si>
   <si>
-    <t>255128a2-2f0e-469b-987c-e68a52b57fd7</t>
+    <t>5b235d20-2d90-4620-8f2b-5645d2987607</t>
   </si>
   <si>
     <t>Gabrvxo</t>
@@ -163,7 +127,7 @@
     <t>j19n2pBr9HyUK3Bq46lBjeYlYIiKpzYv6g0IFH2WbKRFihE</t>
   </si>
   <si>
-    <t>80098f99-6e80-4f33-8c95-26c5889dc678</t>
+    <t>e4aa7ad6-aa02-470e-b5f9-0b9cc7135cbf</t>
   </si>
   <si>
     <t>theKovac</t>
@@ -175,7 +139,7 @@
     <t>kQOTOJNH3Izc_Jzzck4K5Bl4T5VbsMdPYCJoFrG16XNwaw</t>
   </si>
   <si>
-    <t>0b785189-776e-443c-bec9-8447f7150521</t>
+    <t>3128555f-8bc5-428c-afeb-e2ded75bb4b0</t>
   </si>
   <si>
     <t>zRabelo</t>
@@ -567,7 +531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="35" customWidth="1"/>
@@ -616,10 +580,10 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>146</v>
+        <v>248</v>
       </c>
       <c r="E2">
-        <v>4448</v>
+        <v>5012</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -628,10 +592,10 @@
         <v>13</v>
       </c>
       <c r="H2">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="I2">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -645,10 +609,10 @@
         <v>16</v>
       </c>
       <c r="D3">
-        <v>248</v>
+        <v>331</v>
       </c>
       <c r="E3">
-        <v>5012</v>
+        <v>777</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -657,10 +621,10 @@
         <v>13</v>
       </c>
       <c r="H3">
-        <v>46</v>
+        <v>327</v>
       </c>
       <c r="I3">
-        <v>42</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -674,10 +638,10 @@
         <v>20</v>
       </c>
       <c r="D4">
-        <v>222</v>
+        <v>262</v>
       </c>
       <c r="E4">
-        <v>26</v>
+        <v>4897</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
@@ -686,10 +650,10 @@
         <v>13</v>
       </c>
       <c r="H4">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="I4">
-        <v>80</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -703,10 +667,10 @@
         <v>24</v>
       </c>
       <c r="D5">
-        <v>197</v>
+        <v>42</v>
       </c>
       <c r="E5">
-        <v>5028</v>
+        <v>1398</v>
       </c>
       <c r="F5" t="s">
         <v>25</v>
@@ -715,10 +679,10 @@
         <v>13</v>
       </c>
       <c r="H5">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -732,10 +696,10 @@
         <v>28</v>
       </c>
       <c r="D6">
-        <v>331</v>
+        <v>84</v>
       </c>
       <c r="E6">
-        <v>777</v>
+        <v>3836</v>
       </c>
       <c r="F6" t="s">
         <v>29</v>
@@ -744,10 +708,10 @@
         <v>13</v>
       </c>
       <c r="H6">
-        <v>327</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>316</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -761,10 +725,10 @@
         <v>32</v>
       </c>
       <c r="D7">
-        <v>262</v>
+        <v>373</v>
       </c>
       <c r="E7">
-        <v>4897</v>
+        <v>4893</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
@@ -773,10 +737,10 @@
         <v>13</v>
       </c>
       <c r="H7">
-        <v>29</v>
+        <v>184</v>
       </c>
       <c r="I7">
-        <v>26</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -790,10 +754,10 @@
         <v>36</v>
       </c>
       <c r="D8">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E8">
-        <v>1398</v>
+        <v>4397</v>
       </c>
       <c r="F8" t="s">
         <v>37</v>
@@ -819,10 +783,10 @@
         <v>40</v>
       </c>
       <c r="D9">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="E9">
-        <v>3836</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
@@ -848,10 +812,10 @@
         <v>44</v>
       </c>
       <c r="D10">
-        <v>373</v>
+        <v>133</v>
       </c>
       <c r="E10">
-        <v>4893</v>
+        <v>4831</v>
       </c>
       <c r="F10" t="s">
         <v>45</v>
@@ -860,96 +824,9 @@
         <v>13</v>
       </c>
       <c r="H10">
-        <v>184</v>
+        <v>63</v>
       </c>
       <c r="I10">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11">
-        <v>90</v>
-      </c>
-      <c r="E11">
-        <v>4397</v>
-      </c>
-      <c r="F11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12">
-        <v>37</v>
-      </c>
-      <c r="E12">
-        <v>7</v>
-      </c>
-      <c r="F12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13">
-        <v>133</v>
-      </c>
-      <c r="E13">
-        <v>4831</v>
-      </c>
-      <c r="F13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13">
-        <v>63</v>
-      </c>
-      <c r="I13">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Handling errors, Instructions and environment variables
An error handling function was created, which eliminated many lines of code with decision structure. It was also created several more environments for the system to be used in other environments without problems. Updated instructions for handling the API
</commit_message>
<xml_diff>
--- a/res/uploads/Summoners.xlsx
+++ b/res/uploads/Summoners.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -40,7 +40,7 @@
     <t>Losses</t>
   </si>
   <si>
-    <t>2cc9fd5b-a961-43b6-bf0b-9c68960ebbd9</t>
+    <t>4e4a6a37-9b97-4298-8ed4-35ddf1601bd1</t>
   </si>
   <si>
     <t>Old Wolf King</t>
@@ -52,10 +52,10 @@
     <t>ArQcvoAbSEVftDHxS921HN2RMZFL7Sku9OATS98_4KA7GEA</t>
   </si>
   <si>
-    <t>eff810ad-95b8-4a95-9475-d3c0da50bcce</t>
-  </si>
-  <si>
-    <t>888d495a-d2c5-48e3-b19b-7b8979baa2ad</t>
+    <t>c09cdc72-6c50-4ff4-9a9e-5fdbc855e8f3</t>
+  </si>
+  <si>
+    <t>62b8bad1-1fcf-487a-b220-199e1070b10b</t>
   </si>
   <si>
     <t>ThrekSor</t>
@@ -67,7 +67,7 @@
     <t>x5s4POa3xnC9HoXrrz1vvCMjkUj9YBzftuEsrEtrZlnYDQ</t>
   </si>
   <si>
-    <t>5117f20c-14ab-4f55-848f-0720d18aec54</t>
+    <t>8c4abf03-63a4-4879-bd99-9b6be0eea067</t>
   </si>
   <si>
     <t>AndrewDiass</t>
@@ -79,7 +79,7 @@
     <t>ZL-T-dfZdvqgwRyZBp6GzN_H3ZcKL6onpLdkjrRDgg-_w74</t>
   </si>
   <si>
-    <t>3e3e8aba-5d42-4cbc-8b9e-206ead6ab293</t>
+    <t>e4a7f74e-bd07-4e51-ad52-cff71e98d353</t>
   </si>
   <si>
     <t>BiliBoss</t>
@@ -91,7 +91,7 @@
     <t>a_sIcNrytC9otnAGoXxT_WL9ZdL9n-UJYb4KHqX6cYph</t>
   </si>
   <si>
-    <t>3f69ac42-6d11-4597-9215-b14981a84b0e</t>
+    <t>c8cc7c79-ae8b-4651-9054-d6093c81474e</t>
   </si>
   <si>
     <t>DartSecond</t>
@@ -103,7 +103,7 @@
     <t>-WMT4I99JbVdIC3ajBzfYN4C50hxTfR3f--qYJNmtVlMNQ</t>
   </si>
   <si>
-    <t>c566a10b-3992-425c-95a4-df010f1ea34c</t>
+    <t>844a3dd0-a9b6-46b4-929f-177d9076fe27</t>
   </si>
   <si>
     <t>Devils Advocate</t>
@@ -115,7 +115,7 @@
     <t>yN8AgfGPRqBs7z-zwacwmF3W9nQ5IMZBacznV_T4nOVO</t>
   </si>
   <si>
-    <t>5b235d20-2d90-4620-8f2b-5645d2987607</t>
+    <t>6418f889-1a37-411b-aceb-8cd7501d3c82</t>
   </si>
   <si>
     <t>Gabrvxo</t>
@@ -127,7 +127,7 @@
     <t>j19n2pBr9HyUK3Bq46lBjeYlYIiKpzYv6g0IFH2WbKRFihE</t>
   </si>
   <si>
-    <t>e4aa7ad6-aa02-470e-b5f9-0b9cc7135cbf</t>
+    <t>758a38f5-59b0-49d5-9387-c0baa6d35f8d</t>
   </si>
   <si>
     <t>theKovac</t>
@@ -139,7 +139,7 @@
     <t>kQOTOJNH3Izc_Jzzck4K5Bl4T5VbsMdPYCJoFrG16XNwaw</t>
   </si>
   <si>
-    <t>3128555f-8bc5-428c-afeb-e2ded75bb4b0</t>
+    <t>39b5a791-f34a-48d2-9eb7-a85b3e04b6c3</t>
   </si>
   <si>
     <t>zRabelo</t>
@@ -149,6 +149,18 @@
   </si>
   <si>
     <t>Yljd_NnXEx6OgFmZwB6PQ8qYZrBUEaq14DfTCDeHM4sP2h0</t>
+  </si>
+  <si>
+    <t>3db97f18-977c-4821-bf28-b7e255c4b3e1</t>
+  </si>
+  <si>
+    <t>KnifeTheSkull</t>
+  </si>
+  <si>
+    <t>duryWWTOrWpp7wrWyiKPICFY59CvT1W5KfO329u3e6d6vQA</t>
+  </si>
+  <si>
+    <t>SjwN75jquERgi0ch1qfBF06Y-dVtHF5HerErgWj6_2LVbw</t>
   </si>
 </sst>
 </file>
@@ -531,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="35" customWidth="1"/>
@@ -580,10 +592,10 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E2">
-        <v>5012</v>
+        <v>5036</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -592,10 +604,10 @@
         <v>13</v>
       </c>
       <c r="H2">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="I2">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -609,7 +621,7 @@
         <v>16</v>
       </c>
       <c r="D3">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E3">
         <v>777</v>
@@ -621,10 +633,10 @@
         <v>13</v>
       </c>
       <c r="H3">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="I3">
-        <v>316</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -725,10 +737,10 @@
         <v>32</v>
       </c>
       <c r="D7">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="E7">
-        <v>4893</v>
+        <v>657</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
@@ -737,10 +749,10 @@
         <v>13</v>
       </c>
       <c r="H7">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="I7">
-        <v>176</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -828,6 +840,35 @@
       </c>
       <c r="I10">
         <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11">
+        <v>227</v>
+      </c>
+      <c r="E11">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11">
+        <v>90</v>
+      </c>
+      <c r="I11">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>